<commit_message>
Calculate sweep values and clean up
</commit_message>
<xml_diff>
--- a/use_cases/SMR_FT_2023/data/HERON_data.xlsx
+++ b/use_cases/SMR_FT_2023/data/HERON_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/IES_Feb23/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/SMR_FT_2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEF6994-BF94-D64B-ADBF-DC2D3CE21483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A94DB64-9635-D541-AD57-9E1F129A7F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17000" activeTab="4" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="30720" windowHeight="17000" activeTab="6" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="FT" sheetId="11" r:id="rId4"/>
     <sheet name="Boundaries" sheetId="10" r:id="rId5"/>
     <sheet name="Capacity_Market" sheetId="3" r:id="rId6"/>
-    <sheet name="NPP_capacities" sheetId="12" r:id="rId7"/>
+    <sheet name="Tax rates" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="191">
   <si>
     <t>Source</t>
   </si>
@@ -337,27 +337,9 @@
     <t>Capacity negative when component is consuming a resource</t>
   </si>
   <si>
-    <t>Optimized components</t>
-  </si>
-  <si>
-    <t>Lower</t>
-  </si>
-  <si>
-    <t>Upper</t>
-  </si>
-  <si>
-    <t>kg-H2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Capacity  </t>
   </si>
   <si>
-    <t>htse</t>
-  </si>
-  <si>
-    <t>ft</t>
-  </si>
-  <si>
     <t>ft_elec_consumption</t>
   </si>
   <si>
@@ -370,9 +352,6 @@
     <t>naphtha_market</t>
   </si>
   <si>
-    <t>h2_storage</t>
-  </si>
-  <si>
     <t>Update from ANL August 2022</t>
   </si>
   <si>
@@ -460,165 +439,69 @@
     <t>kg-H2/MWh</t>
   </si>
   <si>
-    <t>npp</t>
-  </si>
-  <si>
     <t>elec_market</t>
   </si>
   <si>
-    <t>Elec to H2 rate (HTSE) = 25.13 kg-H2/MWh</t>
-  </si>
-  <si>
-    <t>100 kg initially stored, upper bound ~ 4h of storage for max capacity of FT</t>
-  </si>
-  <si>
-    <t>Plant</t>
-  </si>
-  <si>
     <t>Market</t>
   </si>
   <si>
-    <t>Reactor type</t>
-  </si>
-  <si>
-    <t># Units</t>
-  </si>
-  <si>
-    <t>Capacity (MWth)</t>
-  </si>
-  <si>
-    <t>Capacity (MWe)</t>
-  </si>
-  <si>
     <t>State</t>
   </si>
   <si>
     <t>State corporate income tax rate (%)</t>
   </si>
   <si>
-    <t>Braidwood</t>
-  </si>
-  <si>
     <t>PJM</t>
   </si>
   <si>
-    <t>PWR</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Braidwood_Nuclear_Generating_Station</t>
-  </si>
-  <si>
     <t>Illinois</t>
   </si>
   <si>
-    <t>Davis-Besse</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Davis–Besse_Nuclear_Power_Station</t>
-  </si>
-  <si>
     <t>Ohio</t>
   </si>
   <si>
-    <t>South Texas Project</t>
-  </si>
-  <si>
     <t>ERCOT</t>
   </si>
   <si>
-    <t>https://en.wikipedia.org/wiki/South_Texas_Nuclear_Generating_Station</t>
-  </si>
-  <si>
     <t>Texas</t>
   </si>
   <si>
-    <t>Diablo Canyon</t>
-  </si>
-  <si>
     <t>CAISO</t>
   </si>
   <si>
-    <t>https://en.wikipedia.org/wiki/Diablo_Canyon_Power_Plant</t>
-  </si>
-  <si>
     <t>California</t>
   </si>
   <si>
-    <t>Prairie Island</t>
-  </si>
-  <si>
     <t>MISO</t>
   </si>
   <si>
-    <t>https://en.wikipedia.org/wiki/Prairie_Island_Nuclear_Power_Plant</t>
-  </si>
-  <si>
     <t>Minnesota</t>
   </si>
   <si>
-    <t>Cooper Nuclear Station</t>
-  </si>
-  <si>
     <t>SPP</t>
   </si>
   <si>
-    <t>BWR</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Cooper_Nuclear_Station</t>
-  </si>
-  <si>
     <t>Nebraska</t>
   </si>
   <si>
-    <t>Palo Verde</t>
-  </si>
-  <si>
     <t>Southwest, Arizona</t>
   </si>
   <si>
-    <t>https://en.wikipedia.org/wiki/Palo_Verde_Nuclear_Generating_Station</t>
-  </si>
-  <si>
     <t>Arizona</t>
   </si>
   <si>
-    <t>1194/1160</t>
-  </si>
-  <si>
-    <t>1138/1118</t>
-  </si>
-  <si>
-    <t>522/519</t>
-  </si>
-  <si>
-    <t>1311/1314/1312</t>
-  </si>
-  <si>
     <t>Effective tax rate</t>
   </si>
   <si>
     <t>Federal corporate tax rate</t>
   </si>
   <si>
-    <t>Cooper</t>
-  </si>
-  <si>
     <t>HTSE Lower (MWe)</t>
   </si>
   <si>
-    <t>HTSE Upper (MWe)</t>
-  </si>
-  <si>
     <t>FT Lower (kg-H2)</t>
   </si>
   <si>
-    <t>FT Upper (kg-H2)</t>
-  </si>
-  <si>
-    <t>H2 storage Lower (kg-H2)</t>
-  </si>
-  <si>
     <t>H2 storage Upper (kg-h2)</t>
   </si>
   <si>
@@ -698,6 +581,39 @@
   </si>
   <si>
     <t>Depreciation schedule</t>
+  </si>
+  <si>
+    <t>SMR Capacity (MWe)</t>
+  </si>
+  <si>
+    <t>Storage max capacity (FT prod)</t>
+  </si>
+  <si>
+    <t>48h</t>
+  </si>
+  <si>
+    <t>Case name</t>
+  </si>
+  <si>
+    <t>illinois</t>
+  </si>
+  <si>
+    <t>ohio</t>
+  </si>
+  <si>
+    <t>texas</t>
+  </si>
+  <si>
+    <t>california</t>
+  </si>
+  <si>
+    <t>minnesota</t>
+  </si>
+  <si>
+    <t>nebraska</t>
+  </si>
+  <si>
+    <t>arizona</t>
   </si>
 </sst>
 </file>
@@ -773,7 +689,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -930,6 +846,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -938,7 +874,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -961,8 +897,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
@@ -973,9 +907,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="4" builtinId="4"/>
@@ -2407,10 +2346,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="34"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -2542,7 +2481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926ACCEB-6613-41C3-AB8E-7E632C9D30FD}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -2578,26 +2517,26 @@
       <c r="B4" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -2669,15 +2608,15 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -2755,22 +2694,22 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -2784,11 +2723,11 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -2808,7 +2747,7 @@
         <v>25.125628140703519</v>
       </c>
       <c r="C20" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3009,7 +2948,7 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3024,7 +2963,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
@@ -3038,18 +2977,18 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
-      </c>
-      <c r="M2" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="M2" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="O2" s="27" t="s">
+      <c r="N2" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="O2" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="28" t="s">
+      <c r="P2" s="26" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3057,66 +2996,66 @@
       <c r="B3" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="M3" s="30" t="s">
-        <v>194</v>
+      <c r="M3" s="28" t="s">
+        <v>155</v>
       </c>
       <c r="N3" t="s">
-        <v>195</v>
-      </c>
-      <c r="O3" s="24">
+        <v>156</v>
+      </c>
+      <c r="O3" s="22">
         <v>257800644</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>112</v>
-      </c>
-      <c r="M4" s="30" t="s">
-        <v>197</v>
+        <v>105</v>
+      </c>
+      <c r="M4" s="28" t="s">
+        <v>158</v>
       </c>
       <c r="N4" t="s">
-        <v>198</v>
-      </c>
-      <c r="O4" s="24">
+        <v>159</v>
+      </c>
+      <c r="O4" s="22">
         <v>5156012.88</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B5">
         <v>2019</v>
       </c>
       <c r="H5" t="s">
-        <v>131</v>
-      </c>
-      <c r="M5" s="30"/>
+        <v>124</v>
+      </c>
+      <c r="M5" s="28"/>
       <c r="N5" t="s">
-        <v>199</v>
-      </c>
-      <c r="O5" s="24">
+        <v>160</v>
+      </c>
+      <c r="O5" s="22">
         <v>25780064.399999999</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="H6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="I6">
         <v>100</v>
@@ -3127,20 +3066,20 @@
       <c r="K6">
         <v>1000</v>
       </c>
-      <c r="M6" s="30"/>
+      <c r="M6" s="28"/>
       <c r="N6" t="s">
-        <v>200</v>
-      </c>
-      <c r="O6" s="24">
+        <v>161</v>
+      </c>
+      <c r="O6" s="22">
         <v>38670096.600000001</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B7">
         <v>1.9E-2</v>
@@ -3157,23 +3096,23 @@
       <c r="K7">
         <v>293926000</v>
       </c>
-      <c r="M7" s="30"/>
+      <c r="M7" s="28"/>
       <c r="N7" t="s">
-        <v>201</v>
-      </c>
-      <c r="O7" s="24">
+        <v>162</v>
+      </c>
+      <c r="O7" s="22">
         <v>12251143</v>
       </c>
       <c r="P7" s="14" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="H8" t="s">
         <v>82</v>
@@ -3189,23 +3128,23 @@
         <f>K6/J6</f>
         <v>2.5</v>
       </c>
-      <c r="M8" s="30"/>
+      <c r="M8" s="28"/>
       <c r="N8" t="s">
-        <v>202</v>
-      </c>
-      <c r="O8" s="24">
+        <v>163</v>
+      </c>
+      <c r="O8" s="22">
         <v>38670096.600000001</v>
       </c>
       <c r="P8" s="14" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="H9" t="s">
         <v>83</v>
@@ -3222,19 +3161,19 @@
         <f t="shared" si="0"/>
         <v>0.3979400086720376</v>
       </c>
-      <c r="M9" s="30" t="s">
-        <v>203</v>
-      </c>
-      <c r="O9" s="24">
+      <c r="M9" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="O9" s="22">
         <v>120527413.48</v>
       </c>
       <c r="P9" s="14" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H10" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="I10">
         <f>LOG(I7)</f>
@@ -3248,149 +3187,158 @@
         <f t="shared" si="1"/>
         <v>8.4682380044363352</v>
       </c>
-      <c r="M10" s="30" t="s">
-        <v>204</v>
+      <c r="M10" s="28" t="s">
+        <v>165</v>
       </c>
       <c r="N10" t="s">
-        <v>205</v>
-      </c>
-      <c r="O10" s="24">
+        <v>166</v>
+      </c>
+      <c r="O10" s="22">
         <v>550360</v>
       </c>
       <c r="P10" s="14" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>119</v>
-      </c>
-      <c r="M11" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="31"/>
+      <c r="M11" s="28" t="s">
         <v>81</v>
       </c>
       <c r="N11" t="s">
-        <v>206</v>
-      </c>
-      <c r="O11" s="25">
+        <v>167</v>
+      </c>
+      <c r="O11" s="23">
         <v>378878417.48000002</v>
       </c>
       <c r="P11" s="14" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>123</v>
+      <c r="A12" s="13" t="s">
+        <v>116</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
       </c>
-      <c r="M12" s="30" t="s">
-        <v>207</v>
+      <c r="E12" s="14"/>
+      <c r="M12" s="28" t="s">
+        <v>168</v>
       </c>
       <c r="N12" t="s">
-        <v>208</v>
-      </c>
-      <c r="O12" s="24">
+        <v>169</v>
+      </c>
+      <c r="O12" s="22">
         <v>9607972</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>120</v>
+      <c r="A13" s="13" t="s">
+        <v>113</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
-      </c>
-      <c r="M13" s="30" t="s">
-        <v>210</v>
+        <v>114</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="M13" s="28" t="s">
+        <v>171</v>
       </c>
       <c r="N13" t="s">
-        <v>211</v>
-      </c>
-      <c r="O13" s="24">
+        <v>172</v>
+      </c>
+      <c r="O13" s="22">
         <v>1921594.4</v>
       </c>
       <c r="P13" s="14" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>122</v>
+      <c r="A14" s="13" t="s">
+        <v>115</v>
       </c>
       <c r="B14">
         <v>10625</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D14" t="s">
-        <v>127</v>
-      </c>
-      <c r="M14" s="30" t="s">
-        <v>212</v>
+        <v>120</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="M14" s="28" t="s">
+        <v>173</v>
       </c>
       <c r="N14" t="s">
-        <v>213</v>
-      </c>
-      <c r="O14" s="24">
+        <v>174</v>
+      </c>
+      <c r="O14" s="22">
         <v>7577568.3499999996</v>
       </c>
       <c r="P14" s="14" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>130</v>
+      <c r="A15" s="13" t="s">
+        <v>123</v>
       </c>
       <c r="B15">
         <f>155155000*(1+B7)</f>
         <v>158102945</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="M15" s="30" t="s">
-        <v>214</v>
-      </c>
-      <c r="O15" s="24">
+        <v>130</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="M15" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="O15" s="22">
         <v>1049006</v>
       </c>
       <c r="P15" s="14" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="13" t="s">
         <v>85</v>
       </c>
       <c r="B16">
         <v>0.626</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="M16" s="30" t="s">
-        <v>215</v>
-      </c>
-      <c r="O16" s="25">
+      <c r="E16" s="14"/>
+      <c r="M16" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="O16" s="23">
         <v>20156140.75</v>
       </c>
       <c r="P16" s="14" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="13" t="s">
         <v>86</v>
       </c>
       <c r="B17">
@@ -3399,41 +3347,45 @@
       <c r="C17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M17" s="30" t="s">
-        <v>216</v>
-      </c>
-      <c r="O17" s="24">
+      <c r="E17" s="14"/>
+      <c r="M17" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="O17" s="22">
         <v>7085933</v>
       </c>
       <c r="P17" s="14" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="M18" s="30" t="s">
-        <v>217</v>
-      </c>
-      <c r="O18" s="25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="E18" s="14"/>
+      <c r="M18" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="O18" s="23">
         <v>7085933</v>
       </c>
       <c r="P18" s="14" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>134</v>
+      <c r="A19" s="27" t="s">
+        <v>127</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
-      </c>
-      <c r="M19" s="31" t="s">
-        <v>218</v>
-      </c>
-      <c r="N19" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="M19" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="N19" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="O19" s="26">
+      <c r="O19" s="24">
         <v>20</v>
       </c>
       <c r="P19" s="17" t="s">
@@ -3441,46 +3393,56 @@
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>120</v>
+      <c r="A20" s="13" t="s">
+        <v>113</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
+      <c r="E20" s="14"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>130</v>
-      </c>
-      <c r="B21" s="20">
+      <c r="A21" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="32">
         <f>POWER(1+B7,4)*O18</f>
         <v>7640007.3719816608</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="E21" s="14"/>
+    </row>
+    <row r="22" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="E22" s="14"/>
+    </row>
+    <row r="23" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
         <v>40</v>
       </c>
+      <c r="E23" s="14"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>120</v>
+      <c r="A24" s="13" t="s">
+        <v>113</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>130</v>
-      </c>
-      <c r="B25" s="20">
+      <c r="E24" s="14"/>
+    </row>
+    <row r="25" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="33">
         <f>POWER(1+B7,4)*O16</f>
         <v>21732221.278510533</v>
       </c>
-      <c r="C25" t="s">
-        <v>136</v>
-      </c>
+      <c r="C25" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="24"/>
+      <c r="E25" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3490,17 +3452,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9241F20-95C4-42A2-B03A-23B9DD4DBFA3}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.33203125" customWidth="1"/>
@@ -3508,232 +3472,63 @@
     <col min="12" max="12" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>96</v>
       </c>
       <c r="B1" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G1" t="s">
-        <v>187</v>
-      </c>
-      <c r="H1" t="s">
-        <v>188</v>
-      </c>
-      <c r="I1" t="s">
-        <v>189</v>
-      </c>
-      <c r="J1" t="s">
-        <v>190</v>
-      </c>
-      <c r="K1" t="s">
-        <v>191</v>
-      </c>
-      <c r="L1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>87</v>
       </c>
       <c r="B2" t="s">
         <v>97</v>
       </c>
-      <c r="E2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F2">
-        <v>1194</v>
-      </c>
-      <c r="G2">
-        <f>-F2+14.9</f>
-        <v>-1179.0999999999999</v>
-      </c>
-      <c r="H2">
-        <v>-100</v>
-      </c>
-      <c r="I2">
-        <f>G2*25.13</f>
-        <v>-29630.782999999996</v>
-      </c>
-      <c r="J2">
-        <f>H2*25.13</f>
-        <v>-2513</v>
-      </c>
-      <c r="K2">
-        <f>ABS(I2-25.13*H2)*2</f>
-        <v>54235.565999999992</v>
-      </c>
-      <c r="L2">
-        <f>ABS(I2)*4</f>
-        <v>118523.13199999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>95</v>
       </c>
-      <c r="E3" t="s">
-        <v>156</v>
-      </c>
-      <c r="F3">
-        <v>894</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G8" si="0">-F3+14.9</f>
-        <v>-879.1</v>
-      </c>
-      <c r="H3">
-        <v>-100</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I8" si="1">G3*25.13</f>
-        <v>-22091.782999999999</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J8" si="2">H3*25.13</f>
-        <v>-2513</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K8" si="3">ABS(I3-25.13*H3)*2</f>
-        <v>39157.565999999999</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L8" si="4">ABS(I3)*4</f>
-        <v>88367.131999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" t="s">
-        <v>159</v>
-      </c>
-      <c r="F4">
-        <v>1280</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
-        <v>-1265.0999999999999</v>
-      </c>
-      <c r="H4">
-        <v>-100</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="1"/>
-        <v>-31791.962999999996</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="2"/>
-        <v>-2513</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="3"/>
-        <v>58557.925999999992</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="4"/>
-        <v>127167.85199999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>99</v>
       </c>
       <c r="B5">
-        <v>1193</v>
+        <v>14.9</v>
       </c>
       <c r="C5" t="s">
         <v>66</v>
       </c>
-      <c r="E5" t="s">
-        <v>163</v>
-      </c>
-      <c r="F5">
-        <v>1138</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>-1123.0999999999999</v>
-      </c>
-      <c r="H5">
-        <v>-100</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="1"/>
-        <v>-28223.502999999997</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="2"/>
-        <v>-2513</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="3"/>
-        <v>51421.005999999994</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="4"/>
-        <v>112894.01199999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6">
-        <v>14.9</v>
+        <v>132</v>
+      </c>
+      <c r="B6" s="2">
+        <v>-9.9999999999999997E+199</v>
       </c>
       <c r="C6" t="s">
         <v>66</v>
       </c>
-      <c r="E6" t="s">
-        <v>167</v>
-      </c>
-      <c r="F6">
-        <v>522</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
-        <v>-507.1</v>
-      </c>
-      <c r="H6">
-        <v>-100</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="1"/>
-        <v>-12743.423000000001</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="2"/>
-        <v>-2513</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="3"/>
-        <v>20460.846000000001</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="4"/>
-        <v>50973.692000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="B7" s="2">
         <v>-9.9999999999999997E+199</v>
@@ -3741,39 +3536,10 @@
       <c r="C7" t="s">
         <v>66</v>
       </c>
-      <c r="E7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F7">
-        <v>769</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="0"/>
-        <v>-754.1</v>
-      </c>
-      <c r="H7">
-        <v>-100</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
-        <v>-18950.532999999999</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="2"/>
-        <v>-2513</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="3"/>
-        <v>32875.065999999999</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="4"/>
-        <v>75802.131999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B8" s="2">
         <v>-9.9999999999999997E+199</v>
@@ -3781,39 +3547,10 @@
       <c r="C8" t="s">
         <v>66</v>
       </c>
-      <c r="E8" t="s">
-        <v>176</v>
-      </c>
-      <c r="F8">
-        <v>1314</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>-1299.0999999999999</v>
-      </c>
-      <c r="H8">
-        <v>-100</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
-        <v>-32646.382999999998</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="2"/>
-        <v>-2513</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="3"/>
-        <v>60266.765999999996</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="4"/>
-        <v>130585.53199999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B9" s="2">
         <v>-9.9999999999999997E+199</v>
@@ -3822,104 +3559,114 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="2">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="C10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C14" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B11" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>103</v>
+      <c r="C11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <f>-A12+14.9</f>
+        <v>-45.1</v>
+      </c>
+      <c r="C12" s="35">
+        <f>B12*25.13</f>
+        <v>-1133.3630000000001</v>
+      </c>
+      <c r="D12" s="35">
+        <f>ABS(C12)*48</f>
+        <v>54401.423999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>360</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ref="B13:B16" si="0">-A13+14.9</f>
+        <v>-345.1</v>
+      </c>
+      <c r="C13" s="35">
+        <f>B13*25.13</f>
+        <v>-8672.3629999999994</v>
+      </c>
+      <c r="D13" s="35">
+        <f t="shared" ref="D13:D16" si="1">ABS(C13)*48</f>
+        <v>416273.424</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>720</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>-705.1</v>
+      </c>
+      <c r="C14" s="35">
+        <f>B14*25.13</f>
+        <v>-17719.163</v>
+      </c>
+      <c r="D14" s="35">
+        <f t="shared" si="1"/>
+        <v>850519.82400000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1080</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>-1065.0999999999999</v>
+      </c>
+      <c r="C15" s="35">
+        <f>B15*25.13</f>
+        <v>-26765.962999999996</v>
+      </c>
+      <c r="D15" s="35">
+        <f t="shared" si="1"/>
+        <v>1284766.2239999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1440</v>
       </c>
       <c r="B16">
-        <v>-1175</v>
-      </c>
-      <c r="C16">
-        <v>-100</v>
-      </c>
-      <c r="D16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>104</v>
-      </c>
-      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>-1425.1</v>
+      </c>
+      <c r="C16" s="35">
         <f>B16*25.13</f>
-        <v>-29527.75</v>
-      </c>
-      <c r="C17">
-        <f>C16*25.13</f>
-        <v>-2513</v>
-      </c>
-      <c r="D17" t="s">
-        <v>101</v>
-      </c>
-      <c r="E17" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>-35812.762999999999</v>
+      </c>
+      <c r="D16" s="35">
+        <f t="shared" si="1"/>
+        <v>1719012.6239999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>109</v>
-      </c>
-      <c r="B18">
-        <v>500</v>
-      </c>
-      <c r="C18">
-        <f>ABS(B17)*4</f>
-        <v>118111</v>
-      </c>
-      <c r="D18" t="s">
-        <v>101</v>
-      </c>
-      <c r="E18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>186</v>
+        <v>181</v>
+      </c>
+      <c r="B18" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -4061,304 +3808,173 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5236045A-41A7-AF40-95B6-DBF867B04F6F}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G1" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="21">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="E2" s="19">
+        <f>$B$10+D2*(1-$B$10)</f>
+        <v>0.28505000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="21">
         <v>0</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>3645</v>
-      </c>
-      <c r="F2" t="s">
-        <v>180</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="H2" t="s">
-        <v>155</v>
-      </c>
-      <c r="I2" s="23">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="J2" s="19">
-        <f>$B$10+I2*(1-$B$10)</f>
-        <v>0.28505000000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>2817</v>
-      </c>
-      <c r="F3">
-        <v>894</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="H3" t="s">
-        <v>158</v>
-      </c>
-      <c r="I3" s="23">
+      <c r="E3" s="19">
+        <f t="shared" ref="E3:E8" si="0">$B$10+D3*(1-$B$10)</f>
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D4" s="21">
         <v>0</v>
       </c>
-      <c r="J3" s="19">
-        <f t="shared" ref="J3:J8" si="0">$B$10+I3*(1-$B$10)</f>
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>3853</v>
-      </c>
-      <c r="F4">
-        <v>1280</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="H4" t="s">
-        <v>162</v>
-      </c>
-      <c r="I4" s="23">
-        <v>0</v>
-      </c>
-      <c r="J4" s="19">
+      <c r="E4" s="19">
         <f t="shared" si="0"/>
         <v>0.21</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>3411</v>
-      </c>
-      <c r="F5" t="s">
-        <v>181</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="H5" t="s">
-        <v>166</v>
-      </c>
-      <c r="I5" s="23">
+        <v>142</v>
+      </c>
+      <c r="D5" s="21">
         <v>8.8400000000000006E-2</v>
       </c>
-      <c r="J5" s="19">
+      <c r="E5" s="19">
         <f t="shared" si="0"/>
         <v>0.27983599999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="C6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>1677</v>
-      </c>
-      <c r="F6" t="s">
-        <v>182</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="H6" t="s">
-        <v>170</v>
-      </c>
-      <c r="I6" s="23">
+        <v>144</v>
+      </c>
+      <c r="D6" s="21">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="J6" s="19">
+      <c r="E6" s="19">
         <f t="shared" si="0"/>
         <v>0.28742000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="B7" t="s">
-        <v>172</v>
+        <v>145</v>
       </c>
       <c r="C7" t="s">
-        <v>173</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>2419</v>
-      </c>
-      <c r="F7">
-        <v>769</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="H7" t="s">
-        <v>175</v>
-      </c>
-      <c r="I7" s="23">
+        <v>146</v>
+      </c>
+      <c r="D7" s="21">
         <v>7.8100000000000003E-2</v>
       </c>
-      <c r="J7" s="19">
+      <c r="E7" s="19">
         <f t="shared" si="0"/>
         <v>0.27169900000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="C8" t="s">
-        <v>153</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>3990</v>
-      </c>
-      <c r="F8" t="s">
-        <v>183</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="H8" t="s">
-        <v>179</v>
-      </c>
-      <c r="I8" s="23">
+        <v>148</v>
+      </c>
+      <c r="D8" s="21">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="J8" s="19">
+      <c r="E8" s="19">
         <f t="shared" si="0"/>
         <v>0.24870999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H9" s="18"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9" s="18"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>185</v>
-      </c>
-      <c r="B10" s="22">
+        <v>150</v>
+      </c>
+      <c r="B10" s="20">
         <v>0.21</v>
       </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="18"/>
+      <c r="C10" s="18"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{E420822C-9CB6-0543-ADF1-EDCFE8D5ABAC}"/>
-    <hyperlink ref="G3" r:id="rId2" display="https://en.wikipedia.org/wiki/Davis%E2%80%93Besse_Nuclear_Power_Station" xr:uid="{9110542E-89D6-2D47-BAB0-04E98B13FBF5}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{D1783477-78FF-784B-9A1B-672979000EC5}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{50BD1FBC-1D61-6F40-B26D-85ED74F24A2B}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{3096E627-E5FC-5A4A-BC59-39F664A94478}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{A9BD79D7-5527-A44C-B2EE-3F868C0E23D5}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{9DA2C91F-A18F-F04F-A835-EC8502AD4D48}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>